<commit_message>
Spark SQL query 1
</commit_message>
<xml_diff>
--- a/Documentation/benchmark.xlsx
+++ b/Documentation/benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescomarino/Idea Projects/SABD_project1_BallettiMarino/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FDFF6A-975E-604E-B3BB-AB64016E4BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8724E6D-A493-3E4C-A9A3-DE3B67CC5E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40960" yWindow="-2720" windowWidth="18000" windowHeight="31540" activeTab="5" xr2:uid="{7698990D-6E27-C648-BDDB-21BCFF348DA1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="21160" activeTab="5" xr2:uid="{7698990D-6E27-C648-BDDB-21BCFF348DA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Query 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="8">
   <si>
     <t>Mean:</t>
   </si>
@@ -54,11 +54,23 @@
   <si>
     <t>Execution times (ms)</t>
   </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Solution costs (sum of squared intra cluster distances)</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -83,7 +95,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,6 +111,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -164,12 +182,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
@@ -200,10 +219,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="17" fontId="1" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Colore 2" xfId="1" builtinId="34"/>
     <cellStyle name="20% - Colore 5" xfId="2" builtinId="46"/>
+    <cellStyle name="20% - Colore 6" xfId="3" builtinId="50"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4495,19 +4527,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58DC60B9-AE2E-6548-A2D2-373468EDA4E3}">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A101"/>
+    <sheetView topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -4520,8 +4554,13 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -4533,9 +4572,17 @@
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="17"/>
+      <c r="I2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1611</v>
       </c>
@@ -4554,12 +4601,19 @@
       <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="18">
         <f>AVERAGE(E3:E8)</f>
         <v>3705.6666666666665</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="24">
+        <v>43831</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21">
+        <v>48.827821576647999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>1579</v>
       </c>
@@ -4578,12 +4632,19 @@
       <c r="G4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="18">
         <f>STDEV(E3:E8)</f>
         <v>54.807542060072969</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="24">
+        <v>43862</v>
+      </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21">
+        <v>4.2571098809791801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>1529</v>
       </c>
@@ -4595,9 +4656,16 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="18"/>
+      <c r="I5" s="24">
+        <v>43891</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="21">
+        <v>16343.1927262882</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1470</v>
       </c>
@@ -4609,9 +4677,16 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" s="18"/>
+      <c r="I6" s="24">
+        <v>43922</v>
+      </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21">
+        <v>4128.6979163011702</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>1466</v>
       </c>
@@ -4623,9 +4698,16 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="18"/>
+      <c r="I7" s="24">
+        <v>43952</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21">
+        <v>3820.8464520206699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>1499</v>
       </c>
@@ -4637,9 +4719,12 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" s="18"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>1483</v>
       </c>
@@ -4648,7 +4733,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>1471</v>
       </c>
@@ -4657,7 +4742,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>1458</v>
       </c>
@@ -4666,7 +4751,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>1443</v>
       </c>
@@ -4675,7 +4760,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>1442</v>
       </c>
@@ -4684,7 +4769,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>1435</v>
       </c>
@@ -4693,7 +4778,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>1431</v>
       </c>
@@ -4702,7 +4787,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>1456</v>
       </c>
@@ -5477,9 +5562,10 @@
       <c r="E101" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5487,19 +5573,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE84749-22A5-1347-8A18-58285E063705}">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A101"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -5512,8 +5600,13 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -5526,8 +5619,15 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>831</v>
       </c>
@@ -5550,8 +5650,15 @@
         <f>AVERAGE(E3:E8)</f>
         <v>2973.1666666666665</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="24">
+        <v>43831</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21">
+        <v>48.827821576647999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>811</v>
       </c>
@@ -5574,8 +5681,15 @@
         <f>STDEV(E3:E8)</f>
         <v>80.058520262784441</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="24">
+        <v>43862</v>
+      </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21">
+        <v>4.2190678645824597</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>800</v>
       </c>
@@ -5588,8 +5702,15 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="24">
+        <v>43891</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="21">
+        <v>16343.1927262881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>802</v>
       </c>
@@ -5602,8 +5723,15 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="24">
+        <v>43922</v>
+      </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21">
+        <v>4128.6979163011702</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>801</v>
       </c>
@@ -5616,8 +5744,15 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="24">
+        <v>43952</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21">
+        <v>3820.8464520206699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>799</v>
       </c>
@@ -5630,8 +5765,11 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="25"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>803</v>
       </c>
@@ -5640,7 +5778,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>801</v>
       </c>
@@ -5649,7 +5787,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>806</v>
       </c>
@@ -5658,7 +5796,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>811</v>
       </c>
@@ -5667,7 +5805,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>806</v>
       </c>
@@ -5676,7 +5814,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>816</v>
       </c>
@@ -5685,7 +5823,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>805</v>
       </c>
@@ -5694,7 +5832,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>816</v>
       </c>
@@ -6469,9 +6607,10 @@
       <c r="E101" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Clustering performance comparing completed
</commit_message>
<xml_diff>
--- a/Documentation/benchmark.xlsx
+++ b/Documentation/benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescomarino/Idea Projects/SABD_project1_BallettiMarino/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8724E6D-A493-3E4C-A9A3-DE3B67CC5E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF35D064-B111-7C40-A5C4-7B55BFC11054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="21160" activeTab="5" xr2:uid="{7698990D-6E27-C648-BDDB-21BCFF348DA1}"/>
+    <workbookView xWindow="40960" yWindow="-2720" windowWidth="18000" windowHeight="31540" activeTab="1" xr2:uid="{7698990D-6E27-C648-BDDB-21BCFF348DA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Query 1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -204,6 +204,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="17" fontId="1" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -219,18 +231,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="17" fontId="1" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Colore 2" xfId="1" builtinId="34"/>
@@ -569,18 +569,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -1550,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3568F8A9-1913-3E4A-8996-5367E471A783}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A101"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1564,18 +1564,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -1593,7 +1593,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
-        <v>58</v>
+        <v>935</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="9" t="s">
@@ -1601,10 +1601,10 @@
       </c>
       <c r="D3" s="8">
         <f>AVERAGE(A3:A101)</f>
-        <v>35.484848484848484</v>
+        <v>775.27272727272725</v>
       </c>
       <c r="E3" s="5">
-        <v>3936</v>
+        <v>6452</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="3" t="s">
@@ -1612,12 +1612,12 @@
       </c>
       <c r="H3" s="2">
         <f>AVERAGE(E3:E8)</f>
-        <v>3631.6666666666665</v>
+        <v>6229</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
-        <v>45</v>
+        <v>867</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="9" t="s">
@@ -1625,10 +1625,10 @@
       </c>
       <c r="D4" s="8">
         <f>STDEV(A3:A101)</f>
-        <v>5.3687752496161174</v>
+        <v>24.556398302440975</v>
       </c>
       <c r="E4" s="5">
-        <v>3659</v>
+        <v>6177</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3" t="s">
@@ -1636,18 +1636,18 @@
       </c>
       <c r="H4" s="2">
         <f>STDEV(E3:E8)</f>
-        <v>166.60332129542516</v>
+        <v>147.61436244485157</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <v>49</v>
+        <v>858</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="8"/>
       <c r="E5" s="5">
-        <v>3565</v>
+        <v>6125</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1655,13 +1655,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <v>48</v>
+        <v>825</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="8"/>
       <c r="E6" s="5">
-        <v>3643</v>
+        <v>6377</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1669,13 +1669,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
-        <v>45</v>
+        <v>822</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="8"/>
       <c r="E7" s="5">
-        <v>3530</v>
+        <v>6140</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1683,13 +1683,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <v>40</v>
+        <v>794</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="8"/>
       <c r="E8" s="5">
-        <v>3457</v>
+        <v>6103</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
-        <v>40</v>
+        <v>772</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
-        <v>35</v>
+        <v>790</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
-        <v>40</v>
+        <v>775</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
-        <v>40</v>
+        <v>791</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
-        <v>41</v>
+        <v>758</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
-        <v>34</v>
+        <v>791</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
-        <v>40</v>
+        <v>773</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
-        <v>37</v>
+        <v>760</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
-        <v>40</v>
+        <v>779</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1778,7 +1778,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <v>44</v>
+        <v>797</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <v>36</v>
+        <v>782</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <v>34</v>
+        <v>775</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <v>41</v>
+        <v>780</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <v>33</v>
+        <v>761</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <v>37</v>
+        <v>776</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1832,7 +1832,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <v>35</v>
+        <v>782</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <v>40</v>
+        <v>770</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <v>46</v>
+        <v>769</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <v>39</v>
+        <v>766</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <v>33</v>
+        <v>767</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <v>34</v>
+        <v>774</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <v>32</v>
+        <v>769</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <v>36</v>
+        <v>761</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
-        <v>32</v>
+        <v>781</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
-        <v>38</v>
+        <v>769</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1922,7 +1922,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
-        <v>32</v>
+        <v>778</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <v>34</v>
+        <v>774</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
-        <v>34</v>
+        <v>771</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1949,7 +1949,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
-        <v>34</v>
+        <v>781</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
-        <v>33</v>
+        <v>763</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
-        <v>35</v>
+        <v>758</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
-        <v>32</v>
+        <v>782</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
-        <v>52</v>
+        <v>761</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
-        <v>31</v>
+        <v>756</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
-        <v>34</v>
+        <v>773</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
-        <v>32</v>
+        <v>768</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
-        <v>36</v>
+        <v>755</v>
       </c>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
-        <v>32</v>
+        <v>782</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
-        <v>36</v>
+        <v>767</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -2048,7 +2048,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
-        <v>31</v>
+        <v>774</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -2057,7 +2057,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
-        <v>34</v>
+        <v>758</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
-        <v>33</v>
+        <v>768</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
-        <v>34</v>
+        <v>772</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -2084,7 +2084,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
-        <v>31</v>
+        <v>772</v>
       </c>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
-        <v>37</v>
+        <v>766</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
-        <v>30</v>
+        <v>772</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -2111,7 +2111,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
-        <v>39</v>
+        <v>770</v>
       </c>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
-        <v>31</v>
+        <v>774</v>
       </c>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
-        <v>35</v>
+        <v>760</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
-        <v>31</v>
+        <v>766</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
-        <v>36</v>
+        <v>753</v>
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
-        <v>30</v>
+        <v>760</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
-        <v>34</v>
+        <v>758</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -2174,7 +2174,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
-        <v>31</v>
+        <v>764</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
-        <v>35</v>
+        <v>769</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
-        <v>31</v>
+        <v>750</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -2201,7 +2201,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
-        <v>34</v>
+        <v>774</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -2210,7 +2210,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
-        <v>33</v>
+        <v>784</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
-        <v>36</v>
+        <v>771</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -2228,7 +2228,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
-        <v>31</v>
+        <v>779</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
-        <v>50</v>
+        <v>773</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
-        <v>32</v>
+        <v>765</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
-        <v>34</v>
+        <v>759</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
-        <v>31</v>
+        <v>756</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
-        <v>36</v>
+        <v>761</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
-        <v>32</v>
+        <v>770</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
-        <v>34</v>
+        <v>762</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -2300,7 +2300,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
-        <v>43</v>
+        <v>760</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
-        <v>33</v>
+        <v>772</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
-        <v>32</v>
+        <v>766</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
-        <v>33</v>
+        <v>767</v>
       </c>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
-        <v>31</v>
+        <v>764</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
-        <v>34</v>
+        <v>764</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="6">
-        <v>30</v>
+        <v>784</v>
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
-        <v>34</v>
+        <v>774</v>
       </c>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
-        <v>31</v>
+        <v>758</v>
       </c>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -2381,7 +2381,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="6">
-        <v>34</v>
+        <v>765</v>
       </c>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -2390,7 +2390,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
-        <v>30</v>
+        <v>772</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
-        <v>37</v>
+        <v>772</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -2408,7 +2408,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
-        <v>31</v>
+        <v>765</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
-        <v>34</v>
+        <v>771</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
-        <v>30</v>
+        <v>770</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
-        <v>33</v>
+        <v>828</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
-        <v>30</v>
+        <v>775</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -2453,7 +2453,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
-        <v>34</v>
+        <v>773</v>
       </c>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
-        <v>30</v>
+        <v>767</v>
       </c>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -2471,7 +2471,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
-        <v>32</v>
+        <v>756</v>
       </c>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
-        <v>44</v>
+        <v>766</v>
       </c>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
-        <v>34</v>
+        <v>761</v>
       </c>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
-        <v>30</v>
+        <v>782</v>
       </c>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
-        <v>32</v>
+        <v>768</v>
       </c>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="6">
-        <v>29</v>
+        <v>786</v>
       </c>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
-        <v>33</v>
+        <v>768</v>
       </c>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
@@ -2556,18 +2556,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="12" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -3548,18 +3548,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="12" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -4542,23 +4542,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="12" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="12" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -4572,15 +4572,15 @@
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="22" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="16"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -4601,15 +4601,15 @@
       <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="13">
         <f>AVERAGE(E3:E8)</f>
         <v>3705.6666666666665</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="19">
         <v>43831</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21">
+      <c r="J3" s="15"/>
+      <c r="K3" s="16">
         <v>48.827821576647999</v>
       </c>
     </row>
@@ -4632,15 +4632,15 @@
       <c r="G4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="13">
         <f>STDEV(E3:E8)</f>
         <v>54.807542060072969</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="19">
         <v>43862</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21">
+      <c r="J4" s="15"/>
+      <c r="K4" s="16">
         <v>4.2571098809791801</v>
       </c>
     </row>
@@ -4656,12 +4656,12 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="24">
+      <c r="H5" s="13"/>
+      <c r="I5" s="19">
         <v>43891</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="21">
+      <c r="J5" s="15"/>
+      <c r="K5" s="16">
         <v>16343.1927262882</v>
       </c>
     </row>
@@ -4677,12 +4677,12 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="24">
+      <c r="H6" s="13"/>
+      <c r="I6" s="19">
         <v>43922</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="21">
+      <c r="J6" s="15"/>
+      <c r="K6" s="16">
         <v>4128.6979163011702</v>
       </c>
     </row>
@@ -4698,12 +4698,12 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="24">
+      <c r="H7" s="13"/>
+      <c r="I7" s="19">
         <v>43952</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21">
+      <c r="J7" s="15"/>
+      <c r="K7" s="16">
         <v>3820.8464520206699</v>
       </c>
     </row>
@@ -4719,10 +4719,10 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
@@ -5575,7 +5575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE84749-22A5-1347-8A18-58285E063705}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -5588,23 +5588,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="12" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -5619,11 +5619,11 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="22" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5650,11 +5650,11 @@
         <f>AVERAGE(E3:E8)</f>
         <v>2973.1666666666665</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="19">
         <v>43831</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="21">
+      <c r="J3" s="15"/>
+      <c r="K3" s="16">
         <v>48.827821576647999</v>
       </c>
     </row>
@@ -5681,11 +5681,11 @@
         <f>STDEV(E3:E8)</f>
         <v>80.058520262784441</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="19">
         <v>43862</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="21">
+      <c r="J4" s="15"/>
+      <c r="K4" s="16">
         <v>4.2190678645824597</v>
       </c>
     </row>
@@ -5702,11 +5702,11 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="24">
+      <c r="I5" s="19">
         <v>43891</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="21">
+      <c r="J5" s="15"/>
+      <c r="K5" s="16">
         <v>16343.1927262881</v>
       </c>
     </row>
@@ -5723,11 +5723,11 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="24">
+      <c r="I6" s="19">
         <v>43922</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="21">
+      <c r="J6" s="15"/>
+      <c r="K6" s="16">
         <v>4128.6979163011702</v>
       </c>
     </row>
@@ -5744,11 +5744,11 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="24">
+      <c r="I7" s="19">
         <v>43952</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21">
+      <c r="J7" s="15"/>
+      <c r="K7" s="16">
         <v>3820.8464520206699</v>
       </c>
     </row>
@@ -5765,9 +5765,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="6">

</xml_diff>